<commit_message>
minor edits to vial list file
</commit_message>
<xml_diff>
--- a/NxI_costech_vialList.xlsx
+++ b/NxI_costech_vialList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/NxI_soybean_phys/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{773AFDD2-38C2-0D49-9BCC-578A176174D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A08FF6E-52F0-4649-B7B1-330D925979F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="500" windowWidth="21720" windowHeight="25680" xr2:uid="{DF710A5A-E8E1-A74B-A625-717BFC1E5B71}"/>
+    <workbookView xWindow="18720" yWindow="500" windowWidth="30100" windowHeight="25680" xr2:uid="{DF710A5A-E8E1-A74B-A625-717BFC1E5B71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1285,8 +1285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81C09B7-AB27-9C43-8249-89BF5691B09A}">
   <dimension ref="A1:E289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="E265" sqref="E265"/>
+    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="A283" sqref="A283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5783,7 +5783,7 @@
         <v>6</v>
       </c>
       <c r="E264" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.2">
@@ -5851,7 +5851,7 @@
         <v>7</v>
       </c>
       <c r="E268" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
@@ -5902,7 +5902,7 @@
         <v>7</v>
       </c>
       <c r="E271" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
@@ -5919,7 +5919,7 @@
         <v>7</v>
       </c>
       <c r="E272" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.2">
@@ -5936,7 +5936,7 @@
         <v>7</v>
       </c>
       <c r="E273" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
@@ -5953,7 +5953,7 @@
         <v>7</v>
       </c>
       <c r="E274" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>